<commit_message>
DGTL-106:Done Writing Data in ExcelSheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/BankingGetCredential.xlsx
+++ b/src/test/resources/ExcelSheet/BankingGetCredential.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>mngr473781</t>
+  </si>
   <si>
     <t>vYrysEg</t>
   </si>
@@ -59,15 +62,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="s" s="0">
+      <c r="A1" t="s" s="0">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>